<commit_message>
Enabling all prod testcases for execution
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/Prod/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/Prod/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Master_executors\Prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C4B444-53D7-42CE-B00E-11C9F98AA6C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1882A930-732D-4F9B-80C9-2395CE5DA48A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="65">
   <si>
     <t>Functionality</t>
   </si>
@@ -237,9 +237,6 @@
   <si>
     <t>1. more than 10 Items should be added to cart
 2. Appropriate inventory message must be displayed</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -12113,8 +12110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12160,7 +12157,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>9</v>
@@ -12180,7 +12177,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
@@ -12200,7 +12197,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
@@ -12220,7 +12217,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
@@ -12240,7 +12237,7 @@
         <v>56</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>9</v>
@@ -12260,7 +12257,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
@@ -12280,7 +12277,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>9</v>
@@ -12300,7 +12297,7 @@
         <v>25</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>9</v>
@@ -12320,7 +12317,7 @@
         <v>31</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>9</v>
@@ -12340,7 +12337,7 @@
         <v>33</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>9</v>
@@ -12360,7 +12357,7 @@
         <v>35</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>9</v>
@@ -12380,7 +12377,7 @@
         <v>47</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>9</v>
@@ -12400,7 +12397,7 @@
         <v>37</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>9</v>
@@ -12420,7 +12417,7 @@
         <v>39</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
@@ -12440,7 +12437,7 @@
         <v>41</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>9</v>
@@ -12460,7 +12457,7 @@
         <v>42</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>9</v>
@@ -12480,7 +12477,7 @@
         <v>42</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>9</v>
@@ -12500,7 +12497,7 @@
         <v>45</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
@@ -12520,7 +12517,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>9</v>
@@ -12540,7 +12537,7 @@
         <v>61</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>9</v>
@@ -12560,7 +12557,7 @@
         <v>58</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>9</v>
@@ -12600,7 +12597,7 @@
         <v>22</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>9</v>
@@ -12620,7 +12617,7 @@
         <v>20</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>9</v>
@@ -12640,7 +12637,7 @@
         <v>54</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>9</v>
@@ -12660,7 +12657,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>9</v>
@@ -12680,7 +12677,7 @@
         <v>17</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>9</v>
@@ -12700,7 +12697,7 @@
         <v>64</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>9</v>
@@ -13079,52 +13076,52 @@
   <conditionalFormatting sqref="E3:E6">
     <cfRule type="uniqueValues" dxfId="1014" priority="1015"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1013" priority="1013"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1012" priority="1012"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1011" priority="1011"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1010" priority="1010"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1009" priority="1009"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1008" priority="1008"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1007" priority="1007"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1006" priority="1006"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1005" priority="1005"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1004" priority="1004"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1003" priority="1003"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1002" priority="1002"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1001" priority="1001"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="1000" priority="1000"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="999" priority="999"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="998" priority="1014"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
@@ -13475,52 +13472,52 @@
   <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="882" priority="883"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="881" priority="882"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="880" priority="881"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="879" priority="880"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="878" priority="879"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="877" priority="878"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="876" priority="877"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="875" priority="876"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="874" priority="875"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="873" priority="874"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="872" priority="873"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="871" priority="872"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="870" priority="871"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="869" priority="870"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="868" priority="869"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="867" priority="868"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="866" priority="867"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
@@ -14417,478 +14414,478 @@
   <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="568" priority="569"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="567" priority="568"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="566" priority="567"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="565" priority="566"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="564" priority="565"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="563" priority="564"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="562" priority="563"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="561" priority="562"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="560" priority="561"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="559" priority="560"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="558" priority="559"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="557" priority="558"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="556" priority="557"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="555" priority="556"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="554" priority="555"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="553" priority="554"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="552" priority="553"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="551" priority="552"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="550" priority="551"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="549" priority="550"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="548" priority="549"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="547" priority="548"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="546" priority="547"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="545" priority="546"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="544" priority="545"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="543" priority="544"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="542" priority="543"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="541" priority="542"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="540" priority="541"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="539" priority="540"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="538" priority="539"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="537" priority="538"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="536" priority="537"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="535" priority="536"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="534" priority="535"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="533" priority="534"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="532" priority="533"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="531" priority="532"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="530" priority="531"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="529" priority="530"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="528" priority="529"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="527" priority="528"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="526" priority="527"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="525" priority="526"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="524" priority="525"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="523" priority="524"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="522" priority="523"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="521" priority="522"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="520" priority="521"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="519" priority="520"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="518" priority="519"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="517" priority="517"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="516" priority="516"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="515" priority="515"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="514" priority="514"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="513" priority="513"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="512" priority="512"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="511" priority="511"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="510" priority="510"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="509" priority="509"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="508" priority="508"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="507" priority="507"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="506" priority="506"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="505" priority="505"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="504" priority="504"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="503" priority="503"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="502" priority="518"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="501" priority="502"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="500" priority="501"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="499" priority="500"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="498" priority="499"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="497" priority="498"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="496" priority="497"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="495" priority="496"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="494" priority="495"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="493" priority="494"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="492" priority="493"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="491" priority="492"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="490" priority="491"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="489" priority="490"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="488" priority="489"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="487" priority="488"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="486" priority="487"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="485" priority="486"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="484" priority="485"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="483" priority="484"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="482" priority="483"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="481" priority="482"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="480" priority="481"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="479" priority="480"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="478" priority="479"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="477" priority="478"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="476" priority="477"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="475" priority="476"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="474" priority="475"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="473" priority="474"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="472" priority="473"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="471" priority="472"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="470" priority="471"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="469" priority="470"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="468" priority="469"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="467" priority="468"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="466" priority="467"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="465" priority="466"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="464" priority="465"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="463" priority="464"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="462" priority="463"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="461" priority="462"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="460" priority="461"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="459" priority="460"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="458" priority="459"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="457" priority="458"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="456" priority="457"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="455" priority="456"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="454" priority="455"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="453" priority="454"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="452" priority="453"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="451" priority="452"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="450" priority="451"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="449" priority="450"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="448" priority="449"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="447" priority="448"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="446" priority="447"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="445" priority="446"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="444" priority="445"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="443" priority="444"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="442" priority="443"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="441" priority="441"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="440" priority="440"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="439" priority="439"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="438" priority="438"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="437" priority="437"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="436" priority="436"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="435" priority="435"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="434" priority="434"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="433" priority="433"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="432" priority="432"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="431" priority="431"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="430" priority="430"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="429" priority="429"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="428" priority="428"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="427" priority="427"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="426" priority="442"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="425" priority="426"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="424" priority="425"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="423" priority="424"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="422" priority="423"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="421" priority="422"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="420" priority="421"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="419" priority="420"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="418" priority="419"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="417" priority="418"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="416" priority="417"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="415" priority="416"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="414" priority="415"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="413" priority="414"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="412" priority="413"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="411" priority="412"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E6">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="uniqueValues" dxfId="410" priority="411"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E29">

</xml_diff>

<commit_message>
Disabling TC23 & TC27 for Prod
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/Prod/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/Prod/MasterExecutor_Sanity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LSPL309\Downloads\Updated New TC for  PROD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Master_executors\Prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192B68F9-B5CE-47A8-8727-E2F7F4200293}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2D488E-84CE-472F-9F37-00ED2B53329B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="60">
   <si>
     <t>Functionality</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Verify PDP Page</t>
-  </si>
-  <si>
-    <t>price for listed items should be dispalyed</t>
   </si>
   <si>
     <t>TC02_Serach_Verifications</t>
@@ -169,9 +166,6 @@
     <t>Verify  all Header content</t>
   </si>
   <si>
-    <t>Verify  all Footer content</t>
-  </si>
-  <si>
     <t>1.User should able to perform pagination on PLP
 2.User should able to apply filter on product
 3.User should able to sort products on PLP</t>
@@ -201,9 +195,6 @@
     <t>TC22_Verify_PDP_Page</t>
   </si>
   <si>
-    <t>TC23_Verify_Footer</t>
-  </si>
-  <si>
     <t>TC24_Adding_MultipleItems_QuickOrder</t>
   </si>
   <si>
@@ -211,9 +202,6 @@
   </si>
   <si>
     <t>TC26_Verify_ pagination_SortBy_filteronPLP</t>
-  </si>
-  <si>
-    <t>TC27_Price_Verification_on_CartPage</t>
   </si>
   <si>
     <t>TC08_ Verify_cart_operations</t>
@@ -335,7 +323,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -343,7 +331,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -716,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E28"/>
+      <selection activeCell="C2" sqref="C2:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -758,14 +745,14 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>63</v>
+      <c r="E2" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>9</v>
@@ -779,35 +766,35 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="48.75" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="48.75" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -819,13 +806,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>63</v>
+      <c r="E5" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
@@ -839,13 +826,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>63</v>
+      <c r="E6" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>9</v>
@@ -859,13 +846,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>63</v>
+      <c r="E7" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
@@ -879,35 +866,35 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>63</v>
+      <c r="E8" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45.75" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -919,75 +906,75 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="32.25" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E12" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -995,19 +982,19 @@
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1019,13 +1006,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
@@ -1039,13 +1026,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>63</v>
+      <c r="E16" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>9</v>
@@ -1059,13 +1046,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>63</v>
+      <c r="E17" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>9</v>
@@ -1079,13 +1066,13 @@
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>63</v>
+      <c r="E18" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>9</v>
@@ -1099,13 +1086,13 @@
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="14" t="s">
-        <v>63</v>
+      <c r="E19" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
@@ -1119,13 +1106,13 @@
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>63</v>
+      <c r="E20" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>9</v>
@@ -1138,14 +1125,14 @@
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="11" t="s">
+      <c r="C21" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="14" t="s">
-        <v>63</v>
+      <c r="E21" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>9</v>
@@ -1159,13 +1146,13 @@
         <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>63</v>
+        <v>51</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -1179,115 +1166,75 @@
         <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="37.5" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="D25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="45">
+      <c r="A26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="37.5" customHeight="1">
-      <c r="A25" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="45">
-      <c r="A27" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="D26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TC20 disabled - 18NOV
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/Prod/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/Prod/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Master_executors\Prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2D488E-84CE-472F-9F37-00ED2B53329B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296B02EA-0451-47C2-9196-341D9A658B1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
   <si>
     <t>Functionality</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Verify Find a Branch for GuestUser</t>
-  </si>
-  <si>
-    <t>Verify Find a Branch for loggedinUser</t>
   </si>
   <si>
     <t>User should able to remove item from storeroom</t>
@@ -184,9 +181,6 @@
   </si>
   <si>
     <t>TC19_Verify_ Find_a_Branch_Guestuser</t>
-  </si>
-  <si>
-    <t>TC20_Verify_ Find_a_Branch_Loggedinuser</t>
   </si>
   <si>
     <t>TC21_Verify_Header</t>
@@ -258,7 +252,7 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -323,7 +317,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -347,7 +341,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -703,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -751,8 +744,8 @@
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>59</v>
+      <c r="E2" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>9</v>
@@ -766,13 +759,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>59</v>
+      <c r="E3" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
@@ -786,13 +779,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>59</v>
+      <c r="E4" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>9</v>
@@ -806,13 +799,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>59</v>
+      <c r="E5" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
@@ -826,13 +819,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>59</v>
+      <c r="E6" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>9</v>
@@ -846,13 +839,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>59</v>
+      <c r="E7" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
@@ -866,13 +859,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>59</v>
+      <c r="E8" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>9</v>
@@ -886,13 +879,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>59</v>
+        <v>31</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>9</v>
@@ -906,13 +899,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>59</v>
+      <c r="E10" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>9</v>
@@ -926,13 +919,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>59</v>
+      <c r="E11" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>9</v>
@@ -946,13 +939,13 @@
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>59</v>
+      <c r="E12" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>9</v>
@@ -966,13 +959,13 @@
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>59</v>
+      <c r="E13" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>9</v>
@@ -986,13 +979,13 @@
         <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>59</v>
+      <c r="E14" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>9</v>
@@ -1006,13 +999,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
@@ -1026,13 +1019,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>59</v>
+      <c r="E16" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>9</v>
@@ -1046,13 +1039,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>59</v>
+      <c r="E17" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>9</v>
@@ -1066,13 +1059,13 @@
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>59</v>
+      <c r="E18" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>9</v>
@@ -1086,13 +1079,13 @@
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>59</v>
+      <c r="E19" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
@@ -1106,13 +1099,13 @@
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>59</v>
+      <c r="E20" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>9</v>
@@ -1125,14 +1118,14 @@
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>50</v>
+      <c r="C21" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>59</v>
+        <v>42</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>9</v>
@@ -1146,95 +1139,75 @@
         <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="37.5" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D23" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="45">
+      <c r="A25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="37.5" customHeight="1">
-      <c r="A24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="45">
-      <c r="A26" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" s="5" t="s">
+      <c r="E25" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Disabling TC21 in PROD
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/Prod/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/Prod/MasterExecutor_Sanity.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Master_executors\Prod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KAMAN_SAnity\KAMAN_ECTEST_IE_SANITY\Input_files\Master_executors\Prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296B02EA-0451-47C2-9196-341D9A658B1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="MasterExecutor" sheetId="10" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="56">
   <si>
     <t>Functionality</t>
   </si>
@@ -160,9 +159,6 @@
     <t>Verify user is able to perform all  the Checkout Operations</t>
   </si>
   <si>
-    <t>Verify  all Header content</t>
-  </si>
-  <si>
     <t>1.User should able to perform pagination on PLP
 2.User should able to apply filter on product
 3.User should able to sort products on PLP</t>
@@ -181,9 +177,6 @@
   </si>
   <si>
     <t>TC19_Verify_ Find_a_Branch_Guestuser</t>
-  </si>
-  <si>
-    <t>TC21_Verify_Header</t>
   </si>
   <si>
     <t>TC22_Verify_PDP_Page</t>
@@ -213,7 +206,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -350,9 +343,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 2 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 5" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 3" xfId="3"/>
+    <cellStyle name="Normal 5" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
@@ -695,11 +688,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -745,7 +738,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>9</v>
@@ -765,7 +758,7 @@
         <v>25</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
@@ -785,7 +778,7 @@
         <v>27</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>9</v>
@@ -805,7 +798,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
@@ -825,7 +818,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>9</v>
@@ -845,7 +838,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
@@ -865,7 +858,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>9</v>
@@ -879,13 +872,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>31</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>9</v>
@@ -905,7 +898,7 @@
         <v>34</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>9</v>
@@ -925,7 +918,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>9</v>
@@ -945,7 +938,7 @@
         <v>37</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>9</v>
@@ -965,7 +958,7 @@
         <v>39</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>9</v>
@@ -985,7 +978,7 @@
         <v>41</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>9</v>
@@ -999,13 +992,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
@@ -1019,13 +1012,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>9</v>
@@ -1039,13 +1032,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>9</v>
@@ -1059,13 +1052,13 @@
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>9</v>
@@ -1079,13 +1072,13 @@
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
@@ -1099,13 +1092,13 @@
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>9</v>
@@ -1119,95 +1112,75 @@
         <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="37.5" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D22" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45">
+      <c r="A24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="37.5" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="E24" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="45">
-      <c r="A25" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>